<commit_message>
load all sheets or tables into tabs
</commit_message>
<xml_diff>
--- a/sampledata.xlsx
+++ b/sampledata.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="sampledata" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Another Sheet" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="128">
   <si>
     <t>Region</t>
   </si>
@@ -356,6 +357,45 @@
   </si>
   <si>
     <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Technician</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Actor</t>
   </si>
 </sst>
 </file>
@@ -411,6 +451,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -5065,4 +5109,74 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>